<commit_message>
11.02.2020 mc Sales Details
</commit_message>
<xml_diff>
--- a/2020/Requisition/March/11.03.2020 Requisition of Mughdo Corporation.xlsx
+++ b/2020/Requisition/March/11.03.2020 Requisition of Mughdo Corporation.xlsx
@@ -1081,7 +1081,7 @@
       <pane xSplit="4" ySplit="13" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
-      <selection pane="bottomRight" activeCell="I102" sqref="I102"/>
+      <selection pane="bottomRight" activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21"/>
@@ -1523,11 +1523,11 @@
         <v>721.8</v>
       </c>
       <c r="C9" s="8">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="D9" s="10">
         <f t="shared" si="0"/>
-        <v>101052</v>
+        <v>144360</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>90</v>
@@ -2423,17 +2423,19 @@
       <c r="BU32" s="26"/>
       <c r="BV32" s="26"/>
     </row>
-    <row r="33" spans="1:74" ht="15" hidden="1">
+    <row r="33" spans="1:74" ht="15">
       <c r="A33" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B33" s="9">
         <v>2252.42</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="8">
+        <v>10</v>
+      </c>
       <c r="D33" s="10">
         <f>C33*B33</f>
-        <v>0</v>
+        <v>22524.2</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>90</v>
@@ -2858,20 +2860,22 @@
       </c>
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="1:74" ht="15" hidden="1">
+    <row r="44" spans="1:74" ht="15">
       <c r="A44" s="8" t="s">
         <v>60</v>
       </c>
       <c r="B44" s="9">
         <v>5877.96</v>
       </c>
-      <c r="C44" s="8"/>
+      <c r="C44" s="8">
+        <v>1</v>
+      </c>
       <c r="D44" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5877.96</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>79</v>
+        <v>131</v>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
@@ -4196,19 +4200,17 @@
       <c r="BB93" s="32"/>
       <c r="BC93" s="32"/>
     </row>
-    <row r="94" spans="1:74" ht="14.25" customHeight="1">
+    <row r="94" spans="1:74" ht="14.25" hidden="1" customHeight="1">
       <c r="A94" s="8" t="s">
         <v>115</v>
       </c>
       <c r="B94" s="9">
         <v>7165.02</v>
       </c>
-      <c r="C94" s="8">
-        <v>10</v>
-      </c>
+      <c r="C94" s="8"/>
       <c r="D94" s="10">
         <f t="shared" si="2"/>
-        <v>71650.200000000012</v>
+        <v>0</v>
       </c>
       <c r="E94" s="36" t="s">
         <v>129</v>
@@ -4264,19 +4266,17 @@
       <c r="BB94" s="32"/>
       <c r="BC94" s="32"/>
     </row>
-    <row r="95" spans="1:74" ht="15">
+    <row r="95" spans="1:74" ht="15" hidden="1">
       <c r="A95" s="8" t="s">
         <v>69</v>
       </c>
       <c r="B95" s="9">
         <v>7691.27</v>
       </c>
-      <c r="C95" s="8">
-        <v>5</v>
-      </c>
+      <c r="C95" s="8"/>
       <c r="D95" s="10">
         <f t="shared" si="1"/>
-        <v>38456.350000000006</v>
+        <v>0</v>
       </c>
       <c r="E95" s="36" t="s">
         <v>125</v>
@@ -4351,11 +4351,11 @@
       <c r="B98" s="45"/>
       <c r="C98" s="16">
         <f>SUBTOTAL(9,C9:C97)</f>
-        <v>305</v>
+        <v>361</v>
       </c>
       <c r="D98" s="17">
         <f>SUBTOTAL(9,D9:D97)</f>
-        <v>431398.15</v>
+        <v>393001.76</v>
       </c>
       <c r="E98" s="31"/>
       <c r="F98" s="33"/>

</xml_diff>